<commit_message>
De todo un poco
No entiendo por qué hay versiones repetidas...
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion06/EsqueletoGuion_CS_06_06_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion06/EsqueletoGuion_CS_06_06_CO.xlsx
@@ -13,6 +13,9 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="68">
   <si>
     <t>FICHA</t>
   </si>
@@ -106,39 +109,12 @@
     <t>no</t>
   </si>
   <si>
-    <t>Cultura San Agustín</t>
-  </si>
-  <si>
-    <t>Cultura Tierradentro</t>
-  </si>
-  <si>
-    <t>Importancia de las Culturas Indígenas Doradas.</t>
-  </si>
-  <si>
     <t>Parque Arqueológico de San Agustín</t>
   </si>
   <si>
     <t>si</t>
   </si>
   <si>
-    <t>Períodos históricos de Colombia precolombina.</t>
-  </si>
-  <si>
-    <t>Ubicación geográfica de Los Taironas.</t>
-  </si>
-  <si>
-    <t>Organización social y política Tairona.</t>
-  </si>
-  <si>
-    <t>Generalidades de Los Taironas.</t>
-  </si>
-  <si>
-    <t>Importancia de las Culturas Indígenas Doradas</t>
-  </si>
-  <si>
-    <t>Ubicación geográfica de Los Taironas</t>
-  </si>
-  <si>
     <t>Organización social y política Tairona</t>
   </si>
   <si>
@@ -148,18 +124,9 @@
     <t>El mundo Tairona</t>
   </si>
   <si>
-    <t>Aproximándonos a la cultura Muisca.</t>
-  </si>
-  <si>
-    <t>Aproximándonos a la cultura Muisca</t>
-  </si>
-  <si>
     <t>Generalidades de las Culturas Precolombinas</t>
   </si>
   <si>
-    <t>El crecimiento  y la expansión de los pueblos Caribe.</t>
-  </si>
-  <si>
     <t>Grupos indígenas de la familia Caribe</t>
   </si>
   <si>
@@ -184,21 +151,9 @@
     <t>Conociendo sobre los pueblos precolombinos.</t>
   </si>
   <si>
-    <t>Proyecto: La situación actual de los grupos étnicos en Colombia”.</t>
-  </si>
-  <si>
-    <t>Proyecto: La situación actual de los grupos étnicos en Colombia”</t>
-  </si>
-  <si>
-    <t>Conociendo sobre los pueblos precolombinos</t>
-  </si>
-  <si>
     <t>Competencias: Cuadro comparativo de las culturas indígenas Chibcha, Caribe y Arawak.</t>
   </si>
   <si>
-    <t>Competencias: Cuadro comparativo de las culturas indígenas Chibcha, Caribe y Arawak</t>
-  </si>
-  <si>
     <t>Mapa conceptual</t>
   </si>
   <si>
@@ -226,9 +181,6 @@
     <t>Familias indígenas de Colombia</t>
   </si>
   <si>
-    <t>La familia Chibcha: Tayrona y muiscas</t>
-  </si>
-  <si>
     <t>Destacado</t>
   </si>
   <si>
@@ -242,6 +194,45 @@
   </si>
   <si>
     <t>Fin de tema</t>
+  </si>
+  <si>
+    <t>Periodos históricos de Colombia precolombina</t>
+  </si>
+  <si>
+    <t>La familia Chibcha: taironas y muiscas</t>
+  </si>
+  <si>
+    <t>Taironas</t>
+  </si>
+  <si>
+    <t>Muiscas</t>
+  </si>
+  <si>
+    <t>Origen</t>
+  </si>
+  <si>
+    <t>Pueblos Caribe</t>
+  </si>
+  <si>
+    <t>Otros pueblos Caribe</t>
+  </si>
+  <si>
+    <t>Los Llanos orientales. Otros grupos Arawak</t>
+  </si>
+  <si>
+    <t>Los Achagua</t>
+  </si>
+  <si>
+    <t>Los Piapoco (Yapaco, Cuipaco)</t>
+  </si>
+  <si>
+    <t>Ubicación geográfica de los Taironas</t>
+  </si>
+  <si>
+    <t>Proyecto: La situación actual de los grupos étnicos en Colombia</t>
+  </si>
+  <si>
+    <t>Evaluación sobre Colombia precolombina</t>
   </si>
 </sst>
 </file>
@@ -340,7 +331,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -359,21 +350,6 @@
         <color auto="1"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -825,13 +801,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1251,6 +1227,124 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Hoja1"/>
+      <sheetName val="Hoja2"/>
+      <sheetName val="Hoja3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="107">
+          <cell r="G107" t="str">
+            <v>Periodos históricos de Colombia precolombina</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="G108" t="str">
+            <v>Parque Arqueológico de San Agustín</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="G109" t="str">
+            <v>Periodos históricos de Colombia precolombina</v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="G110" t="str">
+            <v>Ubicación geográfica de los Taironas</v>
+          </cell>
+        </row>
+        <row r="111">
+          <cell r="G111" t="str">
+            <v>Organización social y política Tairona</v>
+          </cell>
+        </row>
+        <row r="112">
+          <cell r="G112" t="str">
+            <v>Generalidades de Los Taironas</v>
+          </cell>
+        </row>
+        <row r="113">
+          <cell r="G113" t="str">
+            <v>El mundo Tairona</v>
+          </cell>
+        </row>
+        <row r="114">
+          <cell r="G114" t="str">
+            <v>Generalidades de las Culturas Precolombinas</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="G115" t="str">
+            <v>Conoce sobre Los Uitotos</v>
+          </cell>
+        </row>
+        <row r="116">
+          <cell r="G116" t="str">
+            <v>El crecimiento  y la expansión de los pueblos Caribe</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="G117" t="str">
+            <v>Grupos indígenas de la familia Caribe</v>
+          </cell>
+        </row>
+        <row r="118">
+          <cell r="G118" t="str">
+            <v>La danza de la Yonna</v>
+          </cell>
+        </row>
+        <row r="119">
+          <cell r="G119" t="str">
+            <v>Los mochilas Wayúu</v>
+          </cell>
+        </row>
+        <row r="120">
+          <cell r="G120" t="str">
+            <v xml:space="preserve">Pueblos Arawak de los Llanos orientales  </v>
+          </cell>
+        </row>
+        <row r="121">
+          <cell r="G121" t="str">
+            <v>Mapa de Lenguas de Colombia</v>
+          </cell>
+        </row>
+        <row r="122">
+          <cell r="G122" t="str">
+            <v>Conociendo sobre los pueblos precolombinos.</v>
+          </cell>
+        </row>
+        <row r="123">
+          <cell r="G123" t="str">
+            <v>Proyecto: La situación actual de los grupos étnicos en Colombia</v>
+          </cell>
+        </row>
+        <row r="124">
+          <cell r="G124" t="str">
+            <v>Competencias: Cuadro comparativo de las culturas indígenas Chibcha, Caribe y Arawak.</v>
+          </cell>
+        </row>
+        <row r="125">
+          <cell r="G125" t="str">
+            <v>Mapa conceptual</v>
+          </cell>
+        </row>
+        <row r="126">
+          <cell r="G126" t="str">
+            <v>Evaluación sobre Colombia precolombina</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -1506,7 +1600,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1664,10 +1758,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A26"/>
+      <selection activeCell="A2" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,8 +1782,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
+      <c r="A2" t="str">
+        <f>[1]Hoja1!G107</f>
+        <v>Periodos históricos de Colombia precolombina</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -1699,8 +1794,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>26</v>
+      <c r="A3" t="str">
+        <f>[1]Hoja1!G108</f>
+        <v>Parque Arqueológico de San Agustín</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -1710,8 +1806,9 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>27</v>
+      <c r="A4" t="str">
+        <f>[1]Hoja1!G109</f>
+        <v>Periodos históricos de Colombia precolombina</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
@@ -1721,8 +1818,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>35</v>
+      <c r="A5" t="str">
+        <f>[1]Hoja1!G110</f>
+        <v>Ubicación geográfica de los Taironas</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -1732,19 +1830,21 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>29</v>
+      <c r="A6" t="str">
+        <f>[1]Hoja1!G111</f>
+        <v>Organización social y política Tairona</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>24</v>
+      <c r="A7" t="str">
+        <f>[1]Hoja1!G112</f>
+        <v>Generalidades de Los Taironas</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -1754,8 +1854,9 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>36</v>
+      <c r="A8" t="str">
+        <f>[1]Hoja1!G113</f>
+        <v>El mundo Tairona</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -1765,8 +1866,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>37</v>
+      <c r="A9" t="str">
+        <f>[1]Hoja1!G114</f>
+        <v>Generalidades de las Culturas Precolombinas</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -1776,8 +1878,9 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>38</v>
+      <c r="A10" t="str">
+        <f>[1]Hoja1!G115</f>
+        <v>Conoce sobre Los Uitotos</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
@@ -1787,8 +1890,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>39</v>
+      <c r="A11" t="str">
+        <f>[1]Hoja1!G116</f>
+        <v>El crecimiento  y la expansión de los pueblos Caribe</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
@@ -1798,8 +1902,9 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>41</v>
+      <c r="A12" t="str">
+        <f>[1]Hoja1!G117</f>
+        <v>Grupos indígenas de la familia Caribe</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -1809,19 +1914,21 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>42</v>
+      <c r="A13" t="str">
+        <f>[1]Hoja1!G118</f>
+        <v>La danza de la Yonna</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>46</v>
+      <c r="A14" t="str">
+        <f>[1]Hoja1!G119</f>
+        <v>Los mochilas Wayúu</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
@@ -1831,8 +1938,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>45</v>
+      <c r="A15" t="str">
+        <f>[1]Hoja1!G120</f>
+        <v xml:space="preserve">Pueblos Arawak de los Llanos orientales  </v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
@@ -1842,8 +1950,9 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>44</v>
+      <c r="A16" t="str">
+        <f>[1]Hoja1!G121</f>
+        <v>Mapa de Lenguas de Colombia</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
@@ -1853,8 +1962,9 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>47</v>
+      <c r="A17" t="str">
+        <f>[1]Hoja1!G122</f>
+        <v>Conociendo sobre los pueblos precolombinos.</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
@@ -1864,19 +1974,21 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>48</v>
+      <c r="A18" t="str">
+        <f>[1]Hoja1!G123</f>
+        <v>Proyecto: La situación actual de los grupos étnicos en Colombia</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>49</v>
+      <c r="A19" t="str">
+        <f>[1]Hoja1!G124</f>
+        <v>Competencias: Cuadro comparativo de las culturas indígenas Chibcha, Caribe y Arawak.</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
@@ -1886,69 +1998,27 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>50</v>
+      <c r="A20" t="str">
+        <f>[1]Hoja1!G125</f>
+        <v>Mapa conceptual</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>54</v>
+      <c r="A21" t="str">
+        <f>[1]Hoja1!G126</f>
+        <v>Evaluación sobre Colombia precolombina</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
       </c>
       <c r="C21">
         <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1973,7 +2043,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2000,7 +2070,7 @@
       </c>
       <c r="B2" t="str">
         <f>'RECURSOS NUEVOS'!A2</f>
-        <v>Períodos históricos de Colombia precolombina</v>
+        <v>Periodos históricos de Colombia precolombina</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>25</v>
@@ -2012,7 +2082,7 @@
       </c>
       <c r="B3" t="str">
         <f>'RECURSOS NUEVOS'!A3</f>
-        <v>Cultura San Agustín</v>
+        <v>Parque Arqueológico de San Agustín</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>25</v>
@@ -2024,7 +2094,7 @@
       </c>
       <c r="B4" t="str">
         <f>'RECURSOS NUEVOS'!A4</f>
-        <v>Cultura Tierradentro</v>
+        <v>Periodos históricos de Colombia precolombina</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>25</v>
@@ -2036,7 +2106,7 @@
       </c>
       <c r="B5" t="str">
         <f>'RECURSOS NUEVOS'!A5</f>
-        <v>Importancia de las Culturas Indígenas Doradas</v>
+        <v>Ubicación geográfica de los Taironas</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>25</v>
@@ -2048,7 +2118,7 @@
       </c>
       <c r="B6" t="str">
         <f>'RECURSOS NUEVOS'!A6</f>
-        <v>Parque Arqueológico de San Agustín</v>
+        <v>Organización social y política Tairona</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>25</v>
@@ -2060,7 +2130,7 @@
       </c>
       <c r="B7" t="str">
         <f>'RECURSOS NUEVOS'!A7</f>
-        <v>Períodos históricos de Colombia precolombina</v>
+        <v>Generalidades de Los Taironas</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>25</v>
@@ -2072,7 +2142,7 @@
       </c>
       <c r="B8" t="str">
         <f>'RECURSOS NUEVOS'!A8</f>
-        <v>Ubicación geográfica de Los Taironas</v>
+        <v>El mundo Tairona</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>25</v>
@@ -2084,7 +2154,7 @@
       </c>
       <c r="B9" t="str">
         <f>'RECURSOS NUEVOS'!A9</f>
-        <v>Organización social y política Tairona</v>
+        <v>Generalidades de las Culturas Precolombinas</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>25</v>
@@ -2096,7 +2166,7 @@
       </c>
       <c r="B10" t="str">
         <f>'RECURSOS NUEVOS'!A10</f>
-        <v>Generalidades de Los Taironas</v>
+        <v>Conoce sobre Los Uitotos</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>25</v>
@@ -2108,7 +2178,7 @@
       </c>
       <c r="B11" t="str">
         <f>'RECURSOS NUEVOS'!A11</f>
-        <v>El mundo Tairona</v>
+        <v>El crecimiento  y la expansión de los pueblos Caribe</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>25</v>
@@ -2120,7 +2190,7 @@
       </c>
       <c r="B12" t="str">
         <f>'RECURSOS NUEVOS'!A12</f>
-        <v>Aproximándonos a la cultura Muisca</v>
+        <v>Grupos indígenas de la familia Caribe</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>25</v>
@@ -2132,7 +2202,7 @@
       </c>
       <c r="B13" t="str">
         <f>'RECURSOS NUEVOS'!A13</f>
-        <v>Generalidades de las Culturas Precolombinas</v>
+        <v>La danza de la Yonna</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>25</v>
@@ -2144,7 +2214,7 @@
       </c>
       <c r="B14" t="str">
         <f>'RECURSOS NUEVOS'!A14</f>
-        <v>Conoce sobre Los Uitotos</v>
+        <v>Los mochilas Wayúu</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>25</v>
@@ -2156,7 +2226,7 @@
       </c>
       <c r="B15" t="str">
         <f>'RECURSOS NUEVOS'!A15</f>
-        <v>El crecimiento  y la expansión de los pueblos Caribe</v>
+        <v xml:space="preserve">Pueblos Arawak de los Llanos orientales  </v>
       </c>
       <c r="C15" s="7" t="s">
         <v>25</v>
@@ -2168,7 +2238,7 @@
       </c>
       <c r="B16" t="str">
         <f>'RECURSOS NUEVOS'!A16</f>
-        <v>Grupos indígenas de la familia Caribe</v>
+        <v>Mapa de Lenguas de Colombia</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>25</v>
@@ -2180,7 +2250,7 @@
       </c>
       <c r="B17" t="str">
         <f>'RECURSOS NUEVOS'!A17</f>
-        <v>La danza de la Yonna</v>
+        <v>Conociendo sobre los pueblos precolombinos.</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>25</v>
@@ -2192,7 +2262,7 @@
       </c>
       <c r="B18" t="str">
         <f>'RECURSOS NUEVOS'!A18</f>
-        <v>Los mochilas Wayúu</v>
+        <v>Proyecto: La situación actual de los grupos étnicos en Colombia</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>25</v>
@@ -2204,7 +2274,7 @@
       </c>
       <c r="B19" t="str">
         <f>'RECURSOS NUEVOS'!A19</f>
-        <v xml:space="preserve">Pueblos Arawak de los Llanos orientales  </v>
+        <v>Competencias: Cuadro comparativo de las culturas indígenas Chibcha, Caribe y Arawak.</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>25</v>
@@ -2216,7 +2286,7 @@
       </c>
       <c r="B20" t="str">
         <f>'RECURSOS NUEVOS'!A20</f>
-        <v>Mapa de Lenguas de Colombia</v>
+        <v>Mapa conceptual</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>25</v>
@@ -2228,57 +2298,9 @@
       </c>
       <c r="B21" t="str">
         <f>'RECURSOS NUEVOS'!A21</f>
-        <v>Conociendo sobre los pueblos precolombinos</v>
+        <v>Evaluación sobre Colombia precolombina</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="str">
-        <f>'RECURSOS NUEVOS'!A22</f>
-        <v>Proyecto: La situación actual de los grupos étnicos en Colombia”</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="str">
-        <f>'RECURSOS NUEVOS'!A23</f>
-        <v>Competencias: Cuadro comparativo de las culturas indígenas Chibcha, Caribe y Arawak</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="str">
-        <f>'RECURSOS NUEVOS'!A24</f>
-        <v>Mapa conceptual</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="str">
-        <f>'RECURSOS NUEVOS'!A25</f>
-        <v>Evaluación</v>
-      </c>
-      <c r="C25" s="7" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2302,10 +2324,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="I85" sqref="I85"/>
+    <sheetView tabSelected="1" topLeftCell="E60" workbookViewId="0">
+      <selection activeCell="I80" sqref="I80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,10 +2375,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
@@ -2373,7 +2395,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
@@ -2390,7 +2412,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
@@ -2407,7 +2429,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
@@ -2424,13 +2446,13 @@
         <v>24</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
+      <c r="H6" s="16"/>
       <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2441,14 +2463,18 @@
         <v>24</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+      <c r="H7" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
@@ -2458,18 +2484,14 @@
         <v>24</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
-      <c r="H8" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
@@ -2479,18 +2501,14 @@
         <v>24</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
-      <c r="H9" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="H9" s="22"/>
+      <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
@@ -2500,18 +2518,14 @@
         <v>24</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
-      <c r="H10" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
@@ -2521,7 +2535,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
@@ -2538,7 +2552,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -2555,7 +2569,7 @@
         <v>24</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
@@ -2572,14 +2586,18 @@
         <v>24</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="H14" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
@@ -2588,11 +2606,13 @@
       <c r="B15" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>43</v>
+      </c>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
       <c r="H15" s="19"/>
@@ -2605,183 +2625,151 @@
       <c r="B16" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>62</v>
-      </c>
+      <c r="C16" s="17"/>
       <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="E16" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="H16" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I20" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>59</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C21" s="8"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="5"/>
+      <c r="G21" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>25</v>
+        <v>49</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2789,10 +2777,10 @@
         <v>19</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2800,10 +2788,10 @@
         <v>19</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2811,10 +2799,10 @@
         <v>19</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2822,10 +2810,10 @@
         <v>19</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2833,10 +2821,16 @@
         <v>19</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2844,10 +2838,16 @@
         <v>19</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2855,10 +2855,16 @@
         <v>19</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2866,10 +2872,13 @@
         <v>19</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2877,50 +2886,32 @@
         <v>19</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H34" t="s">
-        <v>33</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H35" t="s">
-        <v>34</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H36" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>25</v>
+        <v>49</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2928,10 +2919,10 @@
         <v>19</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2939,10 +2930,10 @@
         <v>19</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2950,10 +2941,10 @@
         <v>19</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2961,10 +2952,16 @@
         <v>19</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H40" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2972,10 +2969,16 @@
         <v>19</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H41" t="s">
+        <v>34</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2983,10 +2986,13 @@
         <v>19</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2994,10 +3000,10 @@
         <v>19</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3005,16 +3011,13 @@
         <v>19</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>25</v>
+        <v>49</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3022,13 +3025,13 @@
         <v>19</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="H45" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>25</v>
@@ -3039,10 +3042,13 @@
         <v>19</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3050,13 +3056,10 @@
         <v>19</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3064,10 +3067,10 @@
         <v>19</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3075,10 +3078,10 @@
         <v>19</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3086,16 +3089,10 @@
         <v>19</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H50" t="s">
+        <v>49</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -3103,21 +3100,30 @@
         <v>19</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H51" t="s">
+        <v>32</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -3125,10 +3131,10 @@
         <v>19</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -3136,10 +3142,13 @@
         <v>19</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3147,10 +3156,10 @@
         <v>19</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3158,10 +3167,10 @@
         <v>19</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3169,16 +3178,10 @@
         <v>19</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H57" t="s">
-        <v>43</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3186,10 +3189,10 @@
         <v>19</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3197,10 +3200,10 @@
         <v>19</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3208,13 +3211,10 @@
         <v>19</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3222,10 +3222,10 @@
         <v>19</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3233,10 +3233,10 @@
         <v>19</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3244,10 +3244,16 @@
         <v>19</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>60</v>
+        <v>45</v>
+      </c>
+      <c r="H63" t="s">
+        <v>35</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3255,10 +3261,10 @@
         <v>19</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3266,21 +3272,30 @@
         <v>19</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E65" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H65" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>59</v>
+      <c r="G66" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3288,49 +3303,49 @@
         <v>19</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>19</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>19</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H69" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>19</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3338,16 +3353,10 @@
         <v>19</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H71" t="s">
-        <v>48</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>25</v>
+        <v>49</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3355,10 +3364,10 @@
         <v>19</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3366,10 +3375,16 @@
         <v>19</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H73" t="s">
+        <v>37</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3377,10 +3392,16 @@
         <v>19</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H74" t="s">
+        <v>38</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3388,10 +3409,13 @@
         <v>19</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -3399,43 +3423,57 @@
         <v>19</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>59</v>
+        <v>45</v>
+      </c>
+      <c r="H76" t="s">
+        <v>39</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>19</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H77" t="s">
-        <v>49</v>
-      </c>
-      <c r="I77" s="5" t="s">
+      <c r="A77" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
+      <c r="H77" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I77" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>19</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H78" t="s">
-        <v>50</v>
-      </c>
-      <c r="I78" s="5" t="s">
+      <c r="A78" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C78" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="21"/>
+      <c r="H78" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I78" s="19" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3443,106 +3481,33 @@
       <c r="A79" t="s">
         <v>19</v>
       </c>
-      <c r="B79" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>59</v>
+      <c r="B79" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H79" t="s">
+        <v>41</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>19</v>
       </c>
-      <c r="B80" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>61</v>
+      <c r="B80" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="H80" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B81" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C81" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D81" s="21"/>
-      <c r="E81" s="21"/>
-      <c r="F81" s="21"/>
-      <c r="G81" s="21"/>
-      <c r="H81" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="I81" s="19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B82" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C82" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D82" s="21"/>
-      <c r="E82" s="21"/>
-      <c r="F82" s="21"/>
-      <c r="G82" s="21"/>
-      <c r="H82" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="I82" s="19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>19</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H83" t="s">
-        <v>57</v>
-      </c>
-      <c r="I83" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>19</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H84" t="s">
-        <v>58</v>
-      </c>
-      <c r="I84" s="5" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>